<commit_message>
Fixed the Second Json File
</commit_message>
<xml_diff>
--- a/modifier/English List of districts. Arabic names of districts 2.0.xlsx
+++ b/modifier/English List of districts. Arabic names of districts 2.0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E30DA41-574B-4E2B-AB6F-068354A75C4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EA4C68-391D-4BF7-A2EE-3FE3A3A00843}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arabic To English" sheetId="10" r:id="rId1"/>
@@ -50757,8 +50757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4724775F-9871-41E3-93D1-0001019E1B72}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51143,7 +51143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D60ACC2-503E-4C0B-8735-8409F417B0DE}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>